<commit_message>
adding the clean versions and graphs
</commit_message>
<xml_diff>
--- a/CleanResults/AddedlinksVsRobustness/Results.xlsx
+++ b/CleanResults/AddedlinksVsRobustness/Results.xlsx
@@ -491,7 +491,7 @@
   <dimension ref="A1:I54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4:H54"/>
+      <selection activeCell="D4" sqref="D4:D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1180,6 +1180,18 @@
       <c r="A25" s="3">
         <v>21</v>
       </c>
+      <c r="B25">
+        <v>0.99658725935302395</v>
+      </c>
+      <c r="C25">
+        <v>0.99589069204575498</v>
+      </c>
+      <c r="D25">
+        <v>0.996568721619426</v>
+      </c>
+      <c r="E25">
+        <v>0.99650607378946698</v>
+      </c>
       <c r="F25">
         <v>0.99658725935302395</v>
       </c>
@@ -1197,6 +1209,18 @@
       <c r="A26" s="3">
         <v>22</v>
       </c>
+      <c r="B26">
+        <v>0.99661237757294696</v>
+      </c>
+      <c r="C26">
+        <v>0.99593539809556397</v>
+      </c>
+      <c r="D26">
+        <v>0.99664044862235202</v>
+      </c>
+      <c r="E26">
+        <v>0.99654417917110905</v>
+      </c>
       <c r="F26">
         <v>0.99661237757294696</v>
       </c>
@@ -1214,6 +1238,18 @@
       <c r="A27" s="3">
         <v>23</v>
       </c>
+      <c r="B27">
+        <v>0.99661991424251195</v>
+      </c>
+      <c r="C27">
+        <v>0.99588785757863496</v>
+      </c>
+      <c r="D27">
+        <v>0.99670260684823897</v>
+      </c>
+      <c r="E27">
+        <v>0.99658331526806898</v>
+      </c>
       <c r="F27">
         <v>0.99661991424251195</v>
       </c>
@@ -1231,6 +1267,18 @@
       <c r="A28" s="3">
         <v>24</v>
       </c>
+      <c r="B28">
+        <v>0.99667865832259195</v>
+      </c>
+      <c r="C28">
+        <v>0.99592370683897402</v>
+      </c>
+      <c r="D28">
+        <v>0.99673761517576498</v>
+      </c>
+      <c r="E28">
+        <v>0.99662348208034401</v>
+      </c>
       <c r="F28">
         <v>0.99667865832259195</v>
       </c>
@@ -1248,6 +1296,18 @@
       <c r="A29" s="3">
         <v>25</v>
       </c>
+      <c r="B29">
+        <v>0.996720382940538</v>
+      </c>
+      <c r="C29">
+        <v>0.99595012572346397</v>
+      </c>
+      <c r="D29">
+        <v>0.996776119680719</v>
+      </c>
+      <c r="E29">
+        <v>0.99666260427082698</v>
+      </c>
       <c r="F29">
         <v>0.996720382940538</v>
       </c>
@@ -1265,6 +1325,18 @@
       <c r="A30" s="3">
         <v>26</v>
       </c>
+      <c r="B30">
+        <v>0.99674085297646797</v>
+      </c>
+      <c r="C30">
+        <v>0.99602302510928797</v>
+      </c>
+      <c r="D30">
+        <v>0.99681020690868305</v>
+      </c>
+      <c r="E30">
+        <v>0.99669625496928904</v>
+      </c>
       <c r="F30">
         <v>0.99674085297646797</v>
       </c>
@@ -1282,6 +1354,18 @@
       <c r="A31" s="3">
         <v>27</v>
       </c>
+      <c r="B31">
+        <v>0.99694285317970499</v>
+      </c>
+      <c r="C31">
+        <v>0.99599643101806801</v>
+      </c>
+      <c r="D31">
+        <v>0.99683700486621696</v>
+      </c>
+      <c r="E31">
+        <v>0.99672983011170802</v>
+      </c>
       <c r="F31">
         <v>0.99694285317970499</v>
       </c>
@@ -1299,6 +1383,18 @@
       <c r="A32" s="3">
         <v>28</v>
       </c>
+      <c r="B32">
+        <v>0.99699267693871196</v>
+      </c>
+      <c r="C32">
+        <v>0.99601399980604499</v>
+      </c>
+      <c r="D32">
+        <v>0.99688874209003198</v>
+      </c>
+      <c r="E32">
+        <v>0.99676880587517303</v>
+      </c>
       <c r="F32">
         <v>0.99699267693871196</v>
       </c>
@@ -1316,6 +1412,18 @@
       <c r="A33" s="3">
         <v>29</v>
       </c>
+      <c r="B33">
+        <v>0.99698371179771195</v>
+      </c>
+      <c r="C33">
+        <v>0.996025246055387</v>
+      </c>
+      <c r="D33">
+        <v>0.99691372957420299</v>
+      </c>
+      <c r="E33">
+        <v>0.99680409887645305</v>
+      </c>
       <c r="F33">
         <v>0.99698371179771195</v>
       </c>
@@ -1333,6 +1441,18 @@
       <c r="A34" s="3">
         <v>30</v>
       </c>
+      <c r="B34">
+        <v>0.99700073496099295</v>
+      </c>
+      <c r="C34">
+        <v>0.996066857505162</v>
+      </c>
+      <c r="D34">
+        <v>0.99696767681228804</v>
+      </c>
+      <c r="E34">
+        <v>0.99684484373708004</v>
+      </c>
       <c r="F34">
         <v>0.99700073496099295</v>
       </c>
@@ -1350,6 +1470,18 @@
       <c r="A35" s="3">
         <v>31</v>
       </c>
+      <c r="B35">
+        <v>0.99704837527734103</v>
+      </c>
+      <c r="C35">
+        <v>0.99610583081454296</v>
+      </c>
+      <c r="D35">
+        <v>0.99709948224774203</v>
+      </c>
+      <c r="E35">
+        <v>0.99688454657873105</v>
+      </c>
       <c r="F35">
         <v>0.99704837527734103</v>
       </c>
@@ -1367,6 +1499,18 @@
       <c r="A36" s="3">
         <v>32</v>
       </c>
+      <c r="B36">
+        <v>0.99708926440836598</v>
+      </c>
+      <c r="C36">
+        <v>0.99610908002187404</v>
+      </c>
+      <c r="D36">
+        <v>0.99714867748664004</v>
+      </c>
+      <c r="E36">
+        <v>0.99689989360258202</v>
+      </c>
       <c r="F36">
         <v>0.99708926440836598</v>
       </c>
@@ -1384,6 +1528,18 @@
       <c r="A37" s="3">
         <v>33</v>
       </c>
+      <c r="B37">
+        <v>0.99712520684953398</v>
+      </c>
+      <c r="C37">
+        <v>0.99619732308507103</v>
+      </c>
+      <c r="D37">
+        <v>0.997199885223222</v>
+      </c>
+      <c r="E37">
+        <v>0.99691292724316605</v>
+      </c>
       <c r="F37">
         <v>0.99712520684953398</v>
       </c>
@@ -1401,6 +1557,18 @@
       <c r="A38" s="3">
         <v>34</v>
       </c>
+      <c r="B38">
+        <v>0.99711753835732597</v>
+      </c>
+      <c r="C38">
+        <v>0.99622026958930998</v>
+      </c>
+      <c r="D38">
+        <v>0.99724132243302699</v>
+      </c>
+      <c r="E38">
+        <v>0.99694020951905704</v>
+      </c>
       <c r="F38">
         <v>0.99711753835732597</v>
       </c>
@@ -1418,6 +1586,18 @@
       <c r="A39" s="3">
         <v>35</v>
       </c>
+      <c r="B39">
+        <v>0.99715960953885296</v>
+      </c>
+      <c r="C39">
+        <v>0.99620788709903696</v>
+      </c>
+      <c r="D39">
+        <v>0.99725481089719503</v>
+      </c>
+      <c r="E39">
+        <v>0.99696852251026502</v>
+      </c>
       <c r="F39">
         <v>0.99715960953885296</v>
       </c>
@@ -1435,6 +1615,18 @@
       <c r="A40" s="3">
         <v>36</v>
       </c>
+      <c r="B40">
+        <v>0.99719726991324797</v>
+      </c>
+      <c r="C40">
+        <v>0.99628777980647998</v>
+      </c>
+      <c r="D40">
+        <v>0.99735579563933696</v>
+      </c>
+      <c r="E40">
+        <v>0.99699786621678799</v>
+      </c>
       <c r="F40">
         <v>0.99719726991324797</v>
       </c>
@@ -1452,6 +1644,18 @@
       <c r="A41" s="3">
         <v>37</v>
       </c>
+      <c r="B41">
+        <v>0.99723274533477801</v>
+      </c>
+      <c r="C41">
+        <v>0.99633012748148098</v>
+      </c>
+      <c r="D41">
+        <v>0.99738055162157602</v>
+      </c>
+      <c r="E41">
+        <v>0.99702824063862805</v>
+      </c>
       <c r="F41">
         <v>0.99723274533477801</v>
       </c>
@@ -1469,6 +1673,18 @@
       <c r="A42" s="3">
         <v>38</v>
       </c>
+      <c r="B42">
+        <v>0.99724762935476396</v>
+      </c>
+      <c r="C42">
+        <v>0.99637175365576103</v>
+      </c>
+      <c r="D42">
+        <v>0.99738428101136001</v>
+      </c>
+      <c r="E42">
+        <v>0.99705964577578499</v>
+      </c>
       <c r="F42">
         <v>0.99724762935476396</v>
       </c>
@@ -1486,6 +1702,18 @@
       <c r="A43" s="3">
         <v>39</v>
       </c>
+      <c r="B43">
+        <v>0.99725551759904696</v>
+      </c>
+      <c r="C43">
+        <v>0.99634234145798195</v>
+      </c>
+      <c r="D43">
+        <v>0.99741124566927697</v>
+      </c>
+      <c r="E43">
+        <v>0.99709208162825802</v>
+      </c>
       <c r="F43">
         <v>0.99725551759904696</v>
       </c>
@@ -1503,6 +1731,18 @@
       <c r="A44" s="3">
         <v>40</v>
       </c>
+      <c r="B44">
+        <v>0.99742890206061996</v>
+      </c>
+      <c r="C44">
+        <v>0.99642317653371504</v>
+      </c>
+      <c r="D44">
+        <v>0.99745341010599897</v>
+      </c>
+      <c r="E44">
+        <v>0.99720301815616996</v>
+      </c>
       <c r="F44">
         <v>0.99742890206061996</v>
       </c>
@@ -1520,6 +1760,18 @@
       <c r="A45" s="3">
         <v>41</v>
       </c>
+      <c r="B45">
+        <v>0.99744039453639799</v>
+      </c>
+      <c r="C45">
+        <v>0.99642975593315197</v>
+      </c>
+      <c r="D45">
+        <v>0.99748263348803601</v>
+      </c>
+      <c r="E45">
+        <v>0.99722175289723003</v>
+      </c>
       <c r="F45">
         <v>0.99744039453639799</v>
       </c>
@@ -1537,6 +1789,18 @@
       <c r="A46" s="3">
         <v>42</v>
       </c>
+      <c r="B46">
+        <v>0.99745452024440096</v>
+      </c>
+      <c r="C46">
+        <v>0.99643180263928</v>
+      </c>
+      <c r="D46">
+        <v>0.99749035403657305</v>
+      </c>
+      <c r="E46">
+        <v>0.99728328927880305</v>
+      </c>
       <c r="F46">
         <v>0.99745452024440096</v>
       </c>
@@ -1554,6 +1818,18 @@
       <c r="A47" s="3">
         <v>43</v>
       </c>
+      <c r="B47">
+        <v>0.99746230459912399</v>
+      </c>
+      <c r="C47">
+        <v>0.99655619525346895</v>
+      </c>
+      <c r="D47">
+        <v>0.99749938670206895</v>
+      </c>
+      <c r="E47">
+        <v>0.997315567028768</v>
+      </c>
       <c r="F47">
         <v>0.99746230459912399</v>
       </c>
@@ -1571,6 +1847,18 @@
       <c r="A48" s="3">
         <v>44</v>
       </c>
+      <c r="B48">
+        <v>0.99746346292681298</v>
+      </c>
+      <c r="C48">
+        <v>0.99652310192955895</v>
+      </c>
+      <c r="D48">
+        <v>0.99751377172495703</v>
+      </c>
+      <c r="E48">
+        <v>0.997326822276418</v>
+      </c>
       <c r="F48">
         <v>0.99746346292681298</v>
       </c>
@@ -1588,6 +1876,18 @@
       <c r="A49" s="3">
         <v>45</v>
       </c>
+      <c r="B49">
+        <v>0.99750197895852699</v>
+      </c>
+      <c r="C49">
+        <v>0.99656554776792405</v>
+      </c>
+      <c r="D49">
+        <v>0.99754943038476596</v>
+      </c>
+      <c r="E49">
+        <v>0.99732900760111498</v>
+      </c>
       <c r="F49">
         <v>0.99750197895852699</v>
       </c>
@@ -1605,6 +1905,18 @@
       <c r="A50" s="3">
         <v>46</v>
       </c>
+      <c r="B50">
+        <v>0.99751057234297102</v>
+      </c>
+      <c r="C50">
+        <v>0.99656516493080605</v>
+      </c>
+      <c r="D50">
+        <v>0.99756577785689604</v>
+      </c>
+      <c r="E50">
+        <v>0.99739968685886904</v>
+      </c>
       <c r="F50">
         <v>0.99751057234297102</v>
       </c>
@@ -1622,6 +1934,18 @@
       <c r="A51" s="3">
         <v>47</v>
       </c>
+      <c r="B51">
+        <v>0.997552290954417</v>
+      </c>
+      <c r="C51">
+        <v>0.996689229515756</v>
+      </c>
+      <c r="D51">
+        <v>0.99760743325708601</v>
+      </c>
+      <c r="E51">
+        <v>0.99743465636724604</v>
+      </c>
       <c r="F51">
         <v>0.997552290954417</v>
       </c>
@@ -1639,6 +1963,18 @@
       <c r="A52" s="3">
         <v>48</v>
       </c>
+      <c r="B52">
+        <v>0.99758592417682601</v>
+      </c>
+      <c r="C52">
+        <v>0.99669495980209799</v>
+      </c>
+      <c r="D52">
+        <v>0.99761046895910099</v>
+      </c>
+      <c r="E52">
+        <v>0.997465352943397</v>
+      </c>
       <c r="F52">
         <v>0.99758592417682601</v>
       </c>
@@ -1656,6 +1992,18 @@
       <c r="A53" s="3">
         <v>49</v>
       </c>
+      <c r="B53">
+        <v>0.99760436498268201</v>
+      </c>
+      <c r="C53">
+        <v>0.99669088602251499</v>
+      </c>
+      <c r="D53">
+        <v>0.99762820217071202</v>
+      </c>
+      <c r="E53">
+        <v>0.99746621187282802</v>
+      </c>
       <c r="F53">
         <v>0.99760436498268201</v>
       </c>
@@ -1672,6 +2020,18 @@
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>50</v>
+      </c>
+      <c r="B54">
+        <v>0.99768105838250498</v>
+      </c>
+      <c r="C54">
+        <v>0.99676716795423903</v>
+      </c>
+      <c r="D54">
+        <v>0.99763178022531096</v>
+      </c>
+      <c r="E54">
+        <v>0.99748149263640795</v>
       </c>
       <c r="F54">
         <v>0.99768105838250498</v>

</xml_diff>